<commit_message>
Xử lý lại toàn bộ import
</commit_message>
<xml_diff>
--- a/public/TemplateImport/template_import_faculty.xlsx
+++ b/public/TemplateImport/template_import_faculty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\learning-app\public\TemplateImport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\learning-app\public\TemplateImport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C3001E-2368-4DD0-8028-4AC92BFD8EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FE9F72-76E7-497B-8642-1CDD14468082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{087D9E47-7B34-47D3-8A7D-01AE6CA50FA8}"/>
+    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" xr2:uid="{087D9E47-7B34-47D3-8A7D-01AE6CA50FA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,21 +36,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>ABC</t>
   </si>
   <si>
-    <t xml:space="preserve">Tên Khoa - Chuyên ngành </t>
-  </si>
-  <si>
-    <t>Mã khoa - chuyên ngành</t>
-  </si>
-  <si>
     <t>DEF</t>
   </si>
   <si>
-    <t>KHOA - NGÀNH</t>
+    <t>IMPORT NGÀNH</t>
+  </si>
+  <si>
+    <t>Mã ngành</t>
+  </si>
+  <si>
+    <t>Tên ngành</t>
+  </si>
+  <si>
+    <t>facultyId</t>
+  </si>
+  <si>
+    <t>facultyName</t>
+  </si>
+  <si>
+    <t>creditHourTotal</t>
+  </si>
+  <si>
+    <t>Số tín chỉ của ngành</t>
   </si>
 </sst>
 </file>
@@ -83,8 +95,8 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
-      <color theme="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,7 +110,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -107,49 +119,39 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <bottom style="thick">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -482,44 +484,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DBA273-47A2-4126-A988-E125690B883F}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.85" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="73.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="69.875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="29.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.453125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" ht="39.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" ht="27.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="3" spans="1:3" ht="6.35" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="37.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
+      <c r="C4" s="4">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Điều chỉnh db faculty + major + specialization + bổ sung lưu học kỳ thực hiện
</commit_message>
<xml_diff>
--- a/public/TemplateImport/template_import_faculty.xlsx
+++ b/public/TemplateImport/template_import_faculty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\learning-app\public\TemplateImport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FE9F72-76E7-497B-8642-1CDD14468082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00F84B7-B731-4664-875D-6E2F65D94DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" xr2:uid="{087D9E47-7B34-47D3-8A7D-01AE6CA50FA8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ABC</t>
   </si>
@@ -44,25 +44,19 @@
     <t>DEF</t>
   </si>
   <si>
-    <t>IMPORT NGÀNH</t>
-  </si>
-  <si>
-    <t>Mã ngành</t>
-  </si>
-  <si>
-    <t>Tên ngành</t>
-  </si>
-  <si>
     <t>facultyId</t>
   </si>
   <si>
     <t>facultyName</t>
   </si>
   <si>
-    <t>creditHourTotal</t>
-  </si>
-  <si>
-    <t>Số tín chỉ của ngành</t>
+    <t>IMPORT KHOA</t>
+  </si>
+  <si>
+    <t>Mã khoa</t>
+  </si>
+  <si>
+    <t>Tên khoa</t>
   </si>
 </sst>
 </file>
@@ -484,63 +478,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DBA273-47A2-4126-A988-E125690B883F}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.85" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.6328125" style="1" customWidth="1"/>
     <col min="2" max="2" width="35.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.453125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="1"/>
+    <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="39.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="39.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:2" ht="19.600000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="7.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="27.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="6.35" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="37.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="37.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="C4" s="4">
-        <v>150</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>